<commit_message>
Data set edit 2
</commit_message>
<xml_diff>
--- a/State by State Violations2023.xlsx
+++ b/State by State Violations2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keros\.venv\Capstone-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45F936C-4549-475A-8A77-5E45A83E4DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85150DC0-9A13-4140-8F17-A949B8A4BDF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{05EB7DB3-8D85-4B1D-991F-38359EDF91CB}"/>
+    <workbookView xWindow="28545" yWindow="15480" windowWidth="16410" windowHeight="11295" xr2:uid="{05EB7DB3-8D85-4B1D-991F-38359EDF91CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -420,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0367917-D23D-4C54-B15B-24F602C34A0B}">
-  <dimension ref="B2:J55"/>
+  <dimension ref="B1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,1569 +437,1569 @@
     <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>535</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>52</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="G2">
+        <v>54</v>
+      </c>
+      <c r="H2" s="2">
+        <v>851118</v>
+      </c>
+      <c r="I2" s="2">
+        <v>15761</v>
+      </c>
+      <c r="J2">
         <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>20</v>
-      </c>
-      <c r="C3">
-        <v>535</v>
+        <v>225</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2258</v>
       </c>
       <c r="D3">
+        <v>98</v>
+      </c>
+      <c r="E3">
+        <v>293</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="G3">
+        <v>244</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2078926</v>
+      </c>
+      <c r="I3" s="2">
+        <v>8520</v>
+      </c>
+      <c r="J3">
         <v>9</v>
-      </c>
-      <c r="E3">
-        <v>52</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.88</v>
-      </c>
-      <c r="G3">
-        <v>54</v>
-      </c>
-      <c r="H3" s="2">
-        <v>851118</v>
-      </c>
-      <c r="I3" s="2">
-        <v>15761</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="C4" s="3">
-        <v>2258</v>
+        <v>6039</v>
       </c>
       <c r="D4">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E4">
-        <v>293</v>
+        <v>575</v>
       </c>
       <c r="F4" s="1">
-        <v>0.76</v>
+        <v>0.87</v>
       </c>
       <c r="G4">
-        <v>244</v>
+        <v>346</v>
       </c>
       <c r="H4" s="2">
-        <v>2078926</v>
+        <v>3670366</v>
       </c>
       <c r="I4" s="2">
-        <v>8520</v>
+        <v>10607</v>
       </c>
       <c r="J4">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>218</v>
+        <v>141</v>
       </c>
       <c r="C5" s="3">
-        <v>6039</v>
+        <v>3066</v>
       </c>
       <c r="D5">
-        <v>94</v>
+        <v>9</v>
       </c>
       <c r="E5">
-        <v>575</v>
+        <v>290</v>
       </c>
       <c r="F5" s="1">
-        <v>0.87</v>
+        <v>0.8</v>
       </c>
       <c r="G5">
-        <v>346</v>
+        <v>191</v>
       </c>
       <c r="H5" s="2">
-        <v>3670366</v>
+        <v>1130158</v>
       </c>
       <c r="I5" s="2">
-        <v>10607</v>
+        <v>5917</v>
       </c>
       <c r="J5">
-        <v>26</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>141</v>
+        <v>1169</v>
       </c>
       <c r="C6" s="3">
-        <v>3066</v>
+        <v>52680</v>
       </c>
       <c r="D6">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <v>290</v>
+        <v>480</v>
+      </c>
+      <c r="E6" s="3">
+        <v>5295</v>
       </c>
       <c r="F6" s="1">
-        <v>0.8</v>
+        <v>0.94</v>
       </c>
       <c r="G6">
-        <v>191</v>
+        <v>2765</v>
       </c>
       <c r="H6" s="2">
-        <v>1130158</v>
+        <v>23922459</v>
       </c>
       <c r="I6" s="2">
-        <v>5917</v>
+        <v>8651</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>1169</v>
+        <v>214</v>
       </c>
       <c r="C7" s="3">
-        <v>52680</v>
+        <v>5030</v>
       </c>
       <c r="D7">
-        <v>480</v>
-      </c>
-      <c r="E7" s="3">
-        <v>5295</v>
+        <v>72</v>
+      </c>
+      <c r="E7">
+        <v>448</v>
       </c>
       <c r="F7" s="1">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="G7">
-        <v>2765</v>
+        <v>806</v>
       </c>
       <c r="H7" s="2">
-        <v>23922459</v>
+        <v>10149862</v>
       </c>
       <c r="I7" s="2">
-        <v>8651</v>
+        <v>12592</v>
       </c>
       <c r="J7">
-        <v>123</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="C8" s="3">
-        <v>5030</v>
+        <v>5724</v>
       </c>
       <c r="D8">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E8">
-        <v>448</v>
+        <v>516</v>
       </c>
       <c r="F8" s="1">
-        <v>0.89</v>
+        <v>0.95</v>
       </c>
       <c r="G8">
-        <v>806</v>
+        <v>386</v>
       </c>
       <c r="H8" s="2">
-        <v>10149862</v>
+        <v>6550825</v>
       </c>
       <c r="I8" s="2">
-        <v>12592</v>
+        <v>16971</v>
       </c>
       <c r="J8">
-        <v>32</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>203</v>
-      </c>
-      <c r="C9" s="3">
-        <v>5724</v>
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>896</v>
       </c>
       <c r="D9">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="E9">
-        <v>516</v>
+        <v>68</v>
       </c>
       <c r="F9" s="1">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="G9">
-        <v>386</v>
+        <v>55</v>
       </c>
       <c r="H9" s="2">
-        <v>6550825</v>
+        <v>2412409</v>
       </c>
       <c r="I9" s="2">
-        <v>16971</v>
+        <v>43861</v>
       </c>
       <c r="J9">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>17</v>
-      </c>
-      <c r="C10">
-        <v>896</v>
+        <v>44</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1628</v>
       </c>
       <c r="D10">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E10">
-        <v>68</v>
+        <v>124</v>
       </c>
       <c r="F10" s="1">
-        <v>0.96</v>
+        <v>0.94</v>
       </c>
       <c r="G10">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="H10" s="2">
-        <v>2412409</v>
+        <v>1616516</v>
       </c>
       <c r="I10" s="2">
-        <v>43861</v>
+        <v>22767</v>
       </c>
       <c r="J10">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>44</v>
+        <v>698</v>
       </c>
       <c r="C11" s="3">
-        <v>1628</v>
+        <v>12515</v>
       </c>
       <c r="D11">
-        <v>24</v>
+        <v>554</v>
       </c>
       <c r="E11">
-        <v>124</v>
+        <v>809</v>
       </c>
       <c r="F11" s="1">
-        <v>0.94</v>
+        <v>0.78</v>
       </c>
       <c r="G11">
-        <v>71</v>
+        <v>1542</v>
       </c>
       <c r="H11" s="2">
-        <v>1616516</v>
+        <v>25616117</v>
       </c>
       <c r="I11" s="2">
-        <v>22767</v>
+        <v>16612</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>698</v>
+        <v>357</v>
       </c>
       <c r="C12" s="3">
-        <v>12515</v>
+        <v>4594</v>
       </c>
       <c r="D12">
-        <v>554</v>
+        <v>221</v>
       </c>
       <c r="E12">
-        <v>809</v>
+        <v>422</v>
       </c>
       <c r="F12" s="1">
-        <v>0.78</v>
+        <v>0.85</v>
       </c>
       <c r="G12">
-        <v>1542</v>
+        <v>738</v>
       </c>
       <c r="H12" s="2">
-        <v>25616117</v>
+        <v>8764323</v>
       </c>
       <c r="I12" s="2">
-        <v>16612</v>
+        <v>11875</v>
       </c>
       <c r="J12">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>357</v>
-      </c>
-      <c r="C13" s="3">
-        <v>4594</v>
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>46</v>
       </c>
       <c r="D13">
-        <v>221</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>422</v>
+        <v>6</v>
       </c>
       <c r="F13" s="1">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>738</v>
+        <v>3</v>
       </c>
       <c r="H13" s="2">
-        <v>8764323</v>
+        <v>7150</v>
       </c>
       <c r="I13" s="2">
-        <v>11875</v>
+        <v>2383</v>
       </c>
       <c r="J13">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1365</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E14">
-        <v>6</v>
+        <v>121</v>
       </c>
       <c r="F14" s="1">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="G14">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="H14" s="2">
-        <v>7150</v>
+        <v>2178596</v>
       </c>
       <c r="I14" s="2">
-        <v>2383</v>
+        <v>19279</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>42</v>
+        <v>409</v>
       </c>
       <c r="C15" s="3">
-        <v>1365</v>
+        <v>8519</v>
       </c>
       <c r="D15">
-        <v>20</v>
+        <v>225</v>
       </c>
       <c r="E15">
-        <v>121</v>
+        <v>781</v>
       </c>
       <c r="F15" s="1">
-        <v>0.97</v>
+        <v>0.79</v>
       </c>
       <c r="G15">
-        <v>113</v>
+        <v>946</v>
       </c>
       <c r="H15" s="2">
-        <v>2178596</v>
+        <v>13234798</v>
       </c>
       <c r="I15" s="2">
-        <v>19279</v>
+        <v>13990</v>
       </c>
       <c r="J15">
-        <v>16</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>409</v>
+        <v>81</v>
       </c>
       <c r="C16" s="3">
-        <v>8519</v>
+        <v>2189</v>
       </c>
       <c r="D16">
-        <v>225</v>
+        <v>37</v>
       </c>
       <c r="E16">
-        <v>781</v>
+        <v>205</v>
       </c>
       <c r="F16" s="1">
-        <v>0.79</v>
+        <v>0.73</v>
       </c>
       <c r="G16">
-        <v>946</v>
+        <v>184</v>
       </c>
       <c r="H16" s="2">
-        <v>13234798</v>
+        <v>2486095</v>
       </c>
       <c r="I16" s="2">
-        <v>13990</v>
+        <v>13511</v>
       </c>
       <c r="J16">
-        <v>86</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>81</v>
+        <v>688</v>
       </c>
       <c r="C17" s="3">
-        <v>2189</v>
+        <v>24341</v>
       </c>
       <c r="D17">
-        <v>37</v>
-      </c>
-      <c r="E17">
-        <v>205</v>
+        <v>455</v>
+      </c>
+      <c r="E17" s="3">
+        <v>2243</v>
       </c>
       <c r="F17" s="1">
-        <v>0.73</v>
+        <v>0.84</v>
       </c>
       <c r="G17">
-        <v>184</v>
+        <v>2389</v>
       </c>
       <c r="H17" s="2">
-        <v>2486095</v>
+        <v>69986533</v>
       </c>
       <c r="I17" s="2">
-        <v>13511</v>
+        <v>29295</v>
       </c>
       <c r="J17">
-        <v>8</v>
+        <v>532</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>688</v>
+        <v>518</v>
       </c>
       <c r="C18" s="3">
-        <v>24341</v>
+        <v>14688</v>
       </c>
       <c r="D18">
-        <v>455</v>
+        <v>171</v>
       </c>
       <c r="E18" s="3">
-        <v>2243</v>
+        <v>1580</v>
       </c>
       <c r="F18" s="1">
-        <v>0.84</v>
+        <v>0.78</v>
       </c>
       <c r="G18">
-        <v>2389</v>
+        <v>1325</v>
       </c>
       <c r="H18" s="2">
-        <v>69986533</v>
+        <v>17961843</v>
       </c>
       <c r="I18" s="2">
-        <v>29295</v>
+        <v>13556</v>
       </c>
       <c r="J18">
-        <v>532</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>518</v>
+        <v>311</v>
       </c>
       <c r="C19" s="3">
-        <v>14688</v>
+        <v>7024</v>
       </c>
       <c r="D19">
-        <v>171</v>
-      </c>
-      <c r="E19" s="3">
-        <v>1580</v>
+        <v>220</v>
+      </c>
+      <c r="E19">
+        <v>543</v>
       </c>
       <c r="F19" s="1">
-        <v>0.78</v>
+        <v>0.75</v>
       </c>
       <c r="G19">
-        <v>1325</v>
+        <v>815</v>
       </c>
       <c r="H19" s="2">
-        <v>17961843</v>
+        <v>8183388</v>
       </c>
       <c r="I19" s="2">
-        <v>13556</v>
+        <v>10040</v>
       </c>
       <c r="J19">
-        <v>119</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>311</v>
+        <v>275</v>
       </c>
       <c r="C20" s="3">
-        <v>7024</v>
+        <v>3928</v>
       </c>
       <c r="D20">
-        <v>220</v>
+        <v>341</v>
       </c>
       <c r="E20">
-        <v>543</v>
+        <v>315</v>
       </c>
       <c r="F20" s="1">
-        <v>0.75</v>
+        <v>0.81</v>
       </c>
       <c r="G20">
-        <v>815</v>
+        <v>396</v>
       </c>
       <c r="H20" s="2">
-        <v>8183388</v>
+        <v>8871531</v>
       </c>
       <c r="I20" s="2">
-        <v>10040</v>
+        <v>22402</v>
       </c>
       <c r="J20">
-        <v>68</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C21" s="3">
-        <v>3928</v>
+        <v>4575</v>
       </c>
       <c r="D21">
-        <v>341</v>
+        <v>142</v>
       </c>
       <c r="E21">
-        <v>315</v>
+        <v>465</v>
       </c>
       <c r="F21" s="1">
-        <v>0.81</v>
+        <v>0.82</v>
       </c>
       <c r="G21">
-        <v>396</v>
+        <v>562</v>
       </c>
       <c r="H21" s="2">
-        <v>8871531</v>
+        <v>6286290</v>
       </c>
       <c r="I21" s="2">
-        <v>22402</v>
+        <v>11185</v>
       </c>
       <c r="J21">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>269</v>
+        <v>348</v>
       </c>
       <c r="C22" s="3">
-        <v>4575</v>
+        <v>11350</v>
       </c>
       <c r="D22">
-        <v>142</v>
-      </c>
-      <c r="E22">
-        <v>465</v>
+        <v>62</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1315</v>
       </c>
       <c r="F22" s="1">
-        <v>0.82</v>
+        <v>0.98</v>
       </c>
       <c r="G22">
-        <v>562</v>
+        <v>958</v>
       </c>
       <c r="H22" s="2">
-        <v>6286290</v>
+        <v>20331026</v>
       </c>
       <c r="I22" s="2">
-        <v>11185</v>
+        <v>21222</v>
       </c>
       <c r="J22">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23">
+        <v>225</v>
+      </c>
+      <c r="C23" s="3">
+        <v>9461</v>
+      </c>
+      <c r="D23">
+        <v>72</v>
+      </c>
+      <c r="E23">
+        <v>447</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="G23">
         <v>348</v>
       </c>
-      <c r="C23" s="3">
-        <v>11350</v>
-      </c>
-      <c r="D23">
-        <v>62</v>
-      </c>
-      <c r="E23" s="3">
-        <v>1315</v>
-      </c>
-      <c r="F23" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="G23">
-        <v>958</v>
-      </c>
       <c r="H23" s="2">
-        <v>20331026</v>
+        <v>4825443</v>
       </c>
       <c r="I23" s="2">
-        <v>21222</v>
+        <v>13866</v>
       </c>
       <c r="J23">
-        <v>55</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>225</v>
+        <v>85</v>
       </c>
       <c r="C24" s="3">
-        <v>9461</v>
+        <v>1610</v>
       </c>
       <c r="D24">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="E24">
-        <v>447</v>
+        <v>125</v>
       </c>
       <c r="F24" s="1">
-        <v>0.93</v>
+        <v>0.95</v>
       </c>
       <c r="G24">
-        <v>348</v>
+        <v>89</v>
       </c>
       <c r="H24" s="2">
-        <v>4825443</v>
+        <v>732234</v>
       </c>
       <c r="I24" s="2">
-        <v>13866</v>
+        <v>8227</v>
       </c>
       <c r="J24">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>85</v>
+        <v>427</v>
       </c>
       <c r="C25" s="3">
-        <v>1610</v>
+        <v>16644</v>
       </c>
       <c r="D25">
-        <v>12</v>
-      </c>
-      <c r="E25">
-        <v>125</v>
+        <v>318</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1469</v>
       </c>
       <c r="F25" s="1">
-        <v>0.95</v>
+        <v>0.79</v>
       </c>
       <c r="G25">
-        <v>89</v>
+        <v>1189</v>
       </c>
       <c r="H25" s="2">
-        <v>732234</v>
+        <v>35999121</v>
       </c>
       <c r="I25" s="2">
-        <v>8227</v>
+        <v>30276</v>
       </c>
       <c r="J25">
-        <v>3</v>
+        <v>283</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>427</v>
+        <v>349</v>
       </c>
       <c r="C26" s="3">
-        <v>16644</v>
+        <v>8265</v>
       </c>
       <c r="D26">
-        <v>318</v>
-      </c>
-      <c r="E26" s="3">
-        <v>1469</v>
+        <v>319</v>
+      </c>
+      <c r="E26">
+        <v>919</v>
       </c>
       <c r="F26" s="1">
-        <v>0.79</v>
+        <v>0.82</v>
       </c>
       <c r="G26">
-        <v>1189</v>
+        <v>826</v>
       </c>
       <c r="H26" s="2">
-        <v>35999121</v>
+        <v>14075722</v>
       </c>
       <c r="I26" s="2">
-        <v>30276</v>
+        <v>17040</v>
       </c>
       <c r="J26">
-        <v>283</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27">
-        <v>349</v>
+        <v>506</v>
       </c>
       <c r="C27" s="3">
-        <v>8265</v>
+        <v>15833</v>
       </c>
       <c r="D27">
-        <v>319</v>
-      </c>
-      <c r="E27">
-        <v>919</v>
+        <v>324</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1331</v>
       </c>
       <c r="F27" s="1">
-        <v>0.82</v>
+        <v>0.69</v>
       </c>
       <c r="G27">
-        <v>826</v>
+        <v>1778</v>
       </c>
       <c r="H27" s="2">
-        <v>14075722</v>
+        <v>21549250</v>
       </c>
       <c r="I27" s="2">
-        <v>17040</v>
+        <v>12119</v>
       </c>
       <c r="J27">
-        <v>129</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28">
-        <v>506</v>
+        <v>202</v>
       </c>
       <c r="C28" s="3">
-        <v>15833</v>
+        <v>2634</v>
       </c>
       <c r="D28">
-        <v>324</v>
-      </c>
-      <c r="E28" s="3">
-        <v>1331</v>
+        <v>181</v>
+      </c>
+      <c r="E28">
+        <v>222</v>
       </c>
       <c r="F28" s="1">
-        <v>0.69</v>
+        <v>0.83</v>
       </c>
       <c r="G28">
-        <v>1778</v>
+        <v>227</v>
       </c>
       <c r="H28" s="2">
-        <v>21549250</v>
+        <v>4617342</v>
       </c>
       <c r="I28" s="2">
-        <v>12119</v>
+        <v>20340</v>
       </c>
       <c r="J28">
-        <v>196</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29">
-        <v>202</v>
+        <v>61</v>
       </c>
       <c r="C29" s="3">
-        <v>2634</v>
+        <v>1389</v>
       </c>
       <c r="D29">
-        <v>181</v>
+        <v>27</v>
       </c>
       <c r="E29">
-        <v>222</v>
+        <v>170</v>
       </c>
       <c r="F29" s="1">
-        <v>0.83</v>
+        <v>0.67</v>
       </c>
       <c r="G29">
-        <v>227</v>
+        <v>293</v>
       </c>
       <c r="H29" s="2">
-        <v>4617342</v>
+        <v>4562038</v>
       </c>
       <c r="I29" s="2">
-        <v>20340</v>
+        <v>15570</v>
       </c>
       <c r="J29">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30">
-        <v>61</v>
+        <v>420</v>
       </c>
       <c r="C30" s="3">
-        <v>1389</v>
+        <v>8349</v>
       </c>
       <c r="D30">
-        <v>27</v>
+        <v>397</v>
       </c>
       <c r="E30">
-        <v>170</v>
+        <v>525</v>
       </c>
       <c r="F30" s="1">
-        <v>0.67</v>
+        <v>0.87</v>
       </c>
       <c r="G30">
-        <v>293</v>
+        <v>825</v>
       </c>
       <c r="H30" s="2">
-        <v>4562038</v>
+        <v>22107564</v>
       </c>
       <c r="I30" s="2">
-        <v>15570</v>
+        <v>26797</v>
       </c>
       <c r="J30">
-        <v>12</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31">
-        <v>420</v>
+        <v>76</v>
       </c>
       <c r="C31" s="3">
-        <v>8349</v>
+        <v>1256</v>
       </c>
       <c r="D31">
-        <v>397</v>
+        <v>20</v>
       </c>
       <c r="E31">
-        <v>525</v>
+        <v>137</v>
       </c>
       <c r="F31" s="1">
-        <v>0.87</v>
+        <v>0.79</v>
       </c>
       <c r="G31">
-        <v>825</v>
+        <v>104</v>
       </c>
       <c r="H31" s="2">
-        <v>22107564</v>
+        <v>1146282</v>
       </c>
       <c r="I31" s="2">
-        <v>26797</v>
+        <v>11021</v>
       </c>
       <c r="J31">
-        <v>113</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32">
-        <v>76</v>
+        <v>186</v>
       </c>
       <c r="C32" s="3">
-        <v>1256</v>
+        <v>3744</v>
       </c>
       <c r="D32">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E32">
-        <v>137</v>
+        <v>492</v>
       </c>
       <c r="F32" s="1">
-        <v>0.79</v>
+        <v>0.77</v>
       </c>
       <c r="G32">
-        <v>104</v>
+        <v>369</v>
       </c>
       <c r="H32" s="2">
-        <v>1146282</v>
+        <v>3628833</v>
       </c>
       <c r="I32" s="2">
-        <v>11021</v>
+        <v>9834</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33">
-        <v>186</v>
+        <v>74</v>
       </c>
       <c r="C33" s="3">
-        <v>3744</v>
+        <v>1002</v>
       </c>
       <c r="D33">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="E33">
-        <v>492</v>
+        <v>138</v>
       </c>
       <c r="F33" s="1">
-        <v>0.77</v>
+        <v>0.92</v>
       </c>
       <c r="G33">
-        <v>369</v>
+        <v>95</v>
       </c>
       <c r="H33" s="2">
-        <v>3628833</v>
+        <v>1049582</v>
       </c>
       <c r="I33" s="2">
-        <v>9834</v>
+        <v>11048</v>
       </c>
       <c r="J33">
-        <v>59</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34">
-        <v>74</v>
+        <v>348</v>
       </c>
       <c r="C34" s="3">
-        <v>1002</v>
+        <v>5182</v>
       </c>
       <c r="D34">
-        <v>8</v>
+        <v>130</v>
       </c>
       <c r="E34">
-        <v>138</v>
+        <v>726</v>
       </c>
       <c r="F34" s="1">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="G34">
-        <v>95</v>
+        <v>803</v>
       </c>
       <c r="H34" s="2">
-        <v>1049582</v>
+        <v>12082855</v>
       </c>
       <c r="I34" s="2">
-        <v>11048</v>
+        <v>15047</v>
       </c>
       <c r="J34">
-        <v>2</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35">
-        <v>348</v>
+        <v>68</v>
       </c>
       <c r="C35" s="3">
-        <v>5182</v>
+        <v>2864</v>
       </c>
       <c r="D35">
-        <v>130</v>
+        <v>49</v>
       </c>
       <c r="E35">
-        <v>726</v>
+        <v>241</v>
       </c>
       <c r="F35" s="1">
-        <v>0.93</v>
+        <v>0.85</v>
       </c>
       <c r="G35">
-        <v>803</v>
+        <v>244</v>
       </c>
       <c r="H35" s="2">
-        <v>12082855</v>
+        <v>4624593</v>
       </c>
       <c r="I35" s="2">
-        <v>15047</v>
+        <v>18953</v>
       </c>
       <c r="J35">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C36" s="3">
-        <v>2864</v>
+        <v>2815</v>
       </c>
       <c r="D36">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E36">
-        <v>241</v>
+        <v>259</v>
       </c>
       <c r="F36" s="1">
-        <v>0.85</v>
+        <v>0.87</v>
       </c>
       <c r="G36">
-        <v>244</v>
+        <v>263</v>
       </c>
       <c r="H36" s="2">
-        <v>4624593</v>
+        <v>1479126</v>
       </c>
       <c r="I36" s="2">
-        <v>18953</v>
+        <v>5624</v>
       </c>
       <c r="J36">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37">
-        <v>67</v>
+        <v>606</v>
       </c>
       <c r="C37" s="3">
-        <v>2815</v>
+        <v>9599</v>
       </c>
       <c r="D37">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="E37">
-        <v>259</v>
+        <v>794</v>
       </c>
       <c r="F37" s="1">
-        <v>0.87</v>
+        <v>0.97</v>
       </c>
       <c r="G37">
-        <v>263</v>
+        <v>911</v>
       </c>
       <c r="H37" s="2">
-        <v>1479126</v>
+        <v>7053562</v>
       </c>
       <c r="I37" s="2">
-        <v>5624</v>
+        <v>7742</v>
       </c>
       <c r="J37">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38">
-        <v>606</v>
+        <v>940</v>
       </c>
       <c r="C38" s="3">
-        <v>9599</v>
+        <v>27993</v>
       </c>
       <c r="D38">
-        <v>81</v>
-      </c>
-      <c r="E38">
-        <v>794</v>
+        <v>340</v>
+      </c>
+      <c r="E38" s="3">
+        <v>2507</v>
       </c>
       <c r="F38" s="1">
-        <v>0.97</v>
+        <v>0.72</v>
       </c>
       <c r="G38">
-        <v>911</v>
+        <v>2245</v>
       </c>
       <c r="H38" s="2">
-        <v>7053562</v>
+        <v>35090149</v>
       </c>
       <c r="I38" s="2">
-        <v>7742</v>
+        <v>15630</v>
       </c>
       <c r="J38">
-        <v>20</v>
+        <v>339</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39">
-        <v>940</v>
+        <v>290</v>
       </c>
       <c r="C39" s="3">
-        <v>27993</v>
+        <v>7080</v>
       </c>
       <c r="D39">
-        <v>340</v>
-      </c>
-      <c r="E39" s="3">
-        <v>2507</v>
+        <v>155</v>
+      </c>
+      <c r="E39">
+        <v>641</v>
       </c>
       <c r="F39" s="1">
         <v>0.72</v>
       </c>
       <c r="G39">
-        <v>2245</v>
+        <v>953</v>
       </c>
       <c r="H39" s="2">
-        <v>35090149</v>
+        <v>7787192</v>
       </c>
       <c r="I39" s="2">
-        <v>15630</v>
+        <v>8171</v>
       </c>
       <c r="J39">
-        <v>339</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40">
-        <v>290</v>
+        <v>129</v>
       </c>
       <c r="C40" s="3">
-        <v>7080</v>
+        <v>4557</v>
       </c>
       <c r="D40">
-        <v>155</v>
+        <v>66</v>
       </c>
       <c r="E40">
-        <v>641</v>
+        <v>282</v>
       </c>
       <c r="F40" s="1">
-        <v>0.72</v>
+        <v>0.84</v>
       </c>
       <c r="G40">
-        <v>953</v>
+        <v>313</v>
       </c>
       <c r="H40" s="2">
-        <v>7787192</v>
+        <v>5199588</v>
       </c>
       <c r="I40" s="2">
-        <v>8171</v>
+        <v>16612</v>
       </c>
       <c r="J40">
-        <v>79</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41">
-        <v>129</v>
+        <v>671</v>
       </c>
       <c r="C41" s="3">
-        <v>4557</v>
+        <v>17419</v>
       </c>
       <c r="D41">
-        <v>66</v>
-      </c>
-      <c r="E41">
-        <v>282</v>
+        <v>152</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1222</v>
       </c>
       <c r="F41" s="1">
-        <v>0.84</v>
+        <v>0.85</v>
       </c>
       <c r="G41">
-        <v>313</v>
+        <v>1317</v>
       </c>
       <c r="H41" s="2">
-        <v>5199588</v>
+        <v>21494990</v>
       </c>
       <c r="I41" s="2">
-        <v>16612</v>
+        <v>16321</v>
       </c>
       <c r="J41">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42">
-        <v>671</v>
-      </c>
-      <c r="C42" s="3">
-        <v>17419</v>
+        <v>6</v>
+      </c>
+      <c r="C42">
+        <v>112</v>
       </c>
       <c r="D42">
-        <v>152</v>
-      </c>
-      <c r="E42" s="3">
-        <v>1222</v>
+        <v>3</v>
+      </c>
+      <c r="E42">
+        <v>11</v>
       </c>
       <c r="F42" s="1">
-        <v>0.85</v>
+        <v>0.99</v>
       </c>
       <c r="G42">
-        <v>1317</v>
+        <v>47</v>
       </c>
       <c r="H42" s="2">
-        <v>21494990</v>
+        <v>352025</v>
       </c>
       <c r="I42" s="2">
-        <v>16321</v>
+        <v>7489</v>
       </c>
       <c r="J42">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43">
-        <v>6</v>
-      </c>
-      <c r="C43">
-        <v>112</v>
+        <v>74</v>
+      </c>
+      <c r="C43" s="3">
+        <v>1866</v>
       </c>
       <c r="D43">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="E43">
+        <v>147</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="G43">
+        <v>230</v>
+      </c>
+      <c r="H43" s="2">
+        <v>4727888</v>
+      </c>
+      <c r="I43" s="2">
+        <v>20556</v>
+      </c>
+      <c r="J43">
         <v>11</v>
-      </c>
-      <c r="F43" s="1">
-        <v>0.99</v>
-      </c>
-      <c r="G43">
-        <v>47</v>
-      </c>
-      <c r="H43" s="2">
-        <v>352025</v>
-      </c>
-      <c r="I43" s="2">
-        <v>7489</v>
-      </c>
-      <c r="J43">
-        <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44">
-        <v>74</v>
+        <v>189</v>
       </c>
       <c r="C44" s="3">
-        <v>1866</v>
+        <v>2850</v>
       </c>
       <c r="D44">
-        <v>64</v>
+        <v>116</v>
       </c>
       <c r="E44">
-        <v>147</v>
+        <v>217</v>
       </c>
       <c r="F44" s="1">
-        <v>0.96</v>
+        <v>0.83</v>
       </c>
       <c r="G44">
-        <v>230</v>
+        <v>352</v>
       </c>
       <c r="H44" s="2">
-        <v>4727888</v>
+        <v>4721542</v>
       </c>
       <c r="I44" s="2">
-        <v>20556</v>
+        <v>13413</v>
       </c>
       <c r="J44">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45">
-        <v>189</v>
+        <v>98</v>
       </c>
       <c r="C45" s="3">
-        <v>2850</v>
+        <v>1281</v>
       </c>
       <c r="D45">
-        <v>116</v>
+        <v>20</v>
       </c>
       <c r="E45">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="F45" s="1">
-        <v>0.83</v>
+        <v>0.77</v>
       </c>
       <c r="G45">
-        <v>352</v>
+        <v>163</v>
       </c>
       <c r="H45" s="2">
-        <v>4721542</v>
+        <v>2013213</v>
       </c>
       <c r="I45" s="2">
-        <v>13413</v>
+        <v>12351</v>
       </c>
       <c r="J45">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46">
-        <v>98</v>
+        <v>309</v>
       </c>
       <c r="C46" s="3">
-        <v>1281</v>
+        <v>4309</v>
       </c>
       <c r="D46">
-        <v>20</v>
+        <v>400</v>
       </c>
       <c r="E46">
-        <v>210</v>
+        <v>375</v>
       </c>
       <c r="F46" s="1">
         <v>0.77</v>
       </c>
       <c r="G46">
-        <v>163</v>
+        <v>403</v>
       </c>
       <c r="H46" s="2">
-        <v>2013213</v>
+        <v>9324806</v>
       </c>
       <c r="I46" s="2">
-        <v>12351</v>
+        <v>23138</v>
       </c>
       <c r="J46">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47">
-        <v>309</v>
+        <v>1190</v>
       </c>
       <c r="C47" s="3">
-        <v>4309</v>
+        <v>24058</v>
       </c>
       <c r="D47">
-        <v>400</v>
-      </c>
-      <c r="E47">
-        <v>375</v>
+        <v>941</v>
+      </c>
+      <c r="E47" s="3">
+        <v>2554</v>
       </c>
       <c r="F47" s="1">
-        <v>0.77</v>
+        <v>0.79</v>
       </c>
       <c r="G47">
-        <v>403</v>
+        <v>3592</v>
       </c>
       <c r="H47" s="2">
-        <v>9324806</v>
+        <v>54442591</v>
       </c>
       <c r="I47" s="2">
-        <v>23138</v>
+        <v>15156</v>
       </c>
       <c r="J47">
-        <v>38</v>
+        <v>236</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48">
-        <v>1190</v>
+        <v>98</v>
       </c>
       <c r="C48" s="3">
-        <v>24058</v>
+        <v>2646</v>
       </c>
       <c r="D48">
-        <v>941</v>
-      </c>
-      <c r="E48" s="3">
-        <v>2554</v>
+        <v>40</v>
+      </c>
+      <c r="E48">
+        <v>278</v>
       </c>
       <c r="F48" s="1">
         <v>0.79</v>
       </c>
       <c r="G48">
-        <v>3592</v>
+        <v>275</v>
       </c>
       <c r="H48" s="2">
-        <v>54442591</v>
+        <v>3085350</v>
       </c>
       <c r="I48" s="2">
-        <v>15156</v>
+        <v>11219</v>
       </c>
       <c r="J48">
-        <v>236</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49">
-        <v>98</v>
+        <v>289</v>
       </c>
       <c r="C49" s="3">
-        <v>2646</v>
+        <v>10075</v>
       </c>
       <c r="D49">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="E49">
-        <v>278</v>
+        <v>736</v>
       </c>
       <c r="F49" s="1">
-        <v>0.79</v>
+        <v>0.91</v>
       </c>
       <c r="G49">
-        <v>275</v>
+        <v>459</v>
       </c>
       <c r="H49" s="2">
-        <v>3085350</v>
+        <v>6496163</v>
       </c>
       <c r="I49" s="2">
-        <v>11219</v>
+        <v>14152</v>
       </c>
       <c r="J49">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50">
-        <v>289</v>
-      </c>
-      <c r="C50" s="3">
-        <v>10075</v>
+        <v>34</v>
+      </c>
+      <c r="C50">
+        <v>680</v>
       </c>
       <c r="D50">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="E50">
-        <v>736</v>
+        <v>42</v>
       </c>
       <c r="F50" s="1">
         <v>0.91</v>
       </c>
       <c r="G50">
-        <v>459</v>
+        <v>49</v>
       </c>
       <c r="H50" s="2">
-        <v>6496163</v>
+        <v>1287903</v>
       </c>
       <c r="I50" s="2">
-        <v>14152</v>
+        <v>26283</v>
       </c>
       <c r="J50">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51">
-        <v>34</v>
-      </c>
-      <c r="C51">
-        <v>680</v>
+        <v>195</v>
+      </c>
+      <c r="C51" s="3">
+        <v>10457</v>
       </c>
       <c r="D51">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="E51">
-        <v>42</v>
+        <v>960</v>
       </c>
       <c r="F51" s="1">
-        <v>0.91</v>
+        <v>0.88</v>
       </c>
       <c r="G51">
-        <v>49</v>
+        <v>526</v>
       </c>
       <c r="H51" s="2">
-        <v>1287903</v>
+        <v>14011082</v>
       </c>
       <c r="I51" s="2">
-        <v>26283</v>
+        <v>26637</v>
       </c>
       <c r="J51">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52">
-        <v>195</v>
+        <v>327</v>
       </c>
       <c r="C52" s="3">
-        <v>10457</v>
+        <v>7738</v>
       </c>
       <c r="D52">
-        <v>119</v>
+        <v>270</v>
       </c>
       <c r="E52">
-        <v>960</v>
+        <v>890</v>
       </c>
       <c r="F52" s="1">
-        <v>0.88</v>
+        <v>0.83</v>
       </c>
       <c r="G52">
-        <v>526</v>
+        <v>778</v>
       </c>
       <c r="H52" s="2">
-        <v>14011082</v>
+        <v>19119175</v>
       </c>
       <c r="I52" s="2">
-        <v>26637</v>
+        <v>24574</v>
       </c>
       <c r="J52">
-        <v>36</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53">
-        <v>327</v>
+        <v>122</v>
       </c>
       <c r="C53" s="3">
-        <v>7738</v>
+        <v>4327</v>
       </c>
       <c r="D53">
-        <v>270</v>
+        <v>33</v>
       </c>
       <c r="E53">
-        <v>890</v>
+        <v>346</v>
       </c>
       <c r="F53" s="1">
-        <v>0.83</v>
+        <v>0.89</v>
       </c>
       <c r="G53">
-        <v>778</v>
+        <v>154</v>
       </c>
       <c r="H53" s="2">
-        <v>19119175</v>
+        <v>2557413</v>
       </c>
       <c r="I53" s="2">
-        <v>24574</v>
+        <v>16606</v>
       </c>
       <c r="J53">
-        <v>116</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54">
-        <v>122</v>
-      </c>
-      <c r="C54" s="3">
-        <v>4327</v>
+        <v>35</v>
+      </c>
+      <c r="C54">
+        <v>693</v>
       </c>
       <c r="D54">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="E54">
-        <v>346</v>
+        <v>92</v>
       </c>
       <c r="F54" s="1">
-        <v>0.89</v>
+        <v>0.75</v>
       </c>
       <c r="G54">
-        <v>154</v>
+        <v>102</v>
       </c>
       <c r="H54" s="2">
-        <v>2557413</v>
+        <v>902870</v>
       </c>
       <c r="I54" s="2">
-        <v>16606</v>
+        <v>8851</v>
       </c>
       <c r="J54">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B55">
-        <v>35</v>
-      </c>
-      <c r="C55">
-        <v>693</v>
-      </c>
-      <c r="D55">
-        <v>5</v>
-      </c>
-      <c r="E55">
-        <v>92</v>
-      </c>
-      <c r="F55" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="G55">
-        <v>102</v>
-      </c>
-      <c r="H55" s="2">
-        <v>902870</v>
-      </c>
-      <c r="I55" s="2">
-        <v>8851</v>
-      </c>
-      <c r="J55">
         <v>7</v>
       </c>
     </row>

</xml_diff>